<commit_message>
Use unique document URI's for all test files
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/testResources/SPDXSpreadsheetExample-v2.3.xlsx
+++ b/testResources/SPDXSpreadsheetExample-v2.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary\git\tools-java\testResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3BF6B9-F289-4D2A-9372-956E20237E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54271B05-0BDD-4B4C-BDEE-CFA8EC64ED84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>2.3.0</t>
-  </si>
-  <si>
-    <t>http://spdx.org/spdxdocs/spdx-example-444504E0-4F89-41D3-9A0C-0305E82C3301</t>
   </si>
   <si>
     <t>Package Name</t>
@@ -806,6 +803,9 @@
   </si>
   <si>
     <t>Person: Package Commenter</t>
+  </si>
+  <si>
+    <t>http://spdx.org/spdxdocs/spdx-example-xlsx-2-3-444504E0-4F89-41D3-9A0C-0305E82C3301</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -973,6 +973,7 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,7 +1290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1357,53 +1360,53 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" t="s">
         <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" t="s">
-        <v>81</v>
       </c>
       <c r="L2" s="27">
         <v>40207.771087962959</v>
       </c>
       <c r="M2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="H3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="K4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1439,175 +1442,175 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" t="s">
-        <v>94</v>
       </c>
       <c r="D2"/>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
         <v>95</v>
-      </c>
-      <c r="I2" t="s">
-        <v>96</v>
       </c>
       <c r="J2"/>
       <c r="M2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>94</v>
+      </c>
+      <c r="T2" t="s">
         <v>95</v>
       </c>
-      <c r="N2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>95</v>
-      </c>
-      <c r="T2" t="s">
-        <v>96</v>
-      </c>
       <c r="U2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" t="s">
+        <v>101</v>
+      </c>
+      <c r="O3" t="s">
+        <v>107</v>
+      </c>
+      <c r="P3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q3" t="s">
         <v>99</v>
       </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="R3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" t="s">
         <v>116</v>
       </c>
-      <c r="H3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" t="s">
-        <v>104</v>
-      </c>
-      <c r="L3" t="s">
-        <v>111</v>
-      </c>
-      <c r="M3" t="s">
-        <v>101</v>
-      </c>
-      <c r="N3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P3" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>100</v>
-      </c>
-      <c r="R3" t="s">
-        <v>110</v>
-      </c>
-      <c r="S3" t="s">
-        <v>105</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>117</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>118</v>
-      </c>
-      <c r="W3" t="s">
-        <v>119</v>
       </c>
       <c r="X3" s="28">
         <v>40937.771087962959</v>
@@ -1621,80 +1624,80 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
         <v>120</v>
       </c>
-      <c r="B4" t="s">
-        <v>121</v>
-      </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4"/>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4"/>
       <c r="M4"/>
       <c r="N4"/>
       <c r="Q4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
         <v>125</v>
       </c>
-      <c r="B5" t="s">
-        <v>126</v>
-      </c>
       <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
         <v>134</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" t="s">
         <v>130</v>
-      </c>
-      <c r="G5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I5" t="s">
-        <v>131</v>
       </c>
       <c r="J5"/>
       <c r="M5" t="s">
+        <v>127</v>
+      </c>
+      <c r="N5" t="s">
+        <v>127</v>
+      </c>
+      <c r="P5" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>126</v>
+      </c>
+      <c r="S5" t="s">
         <v>128</v>
       </c>
-      <c r="N5" t="s">
-        <v>128</v>
-      </c>
-      <c r="P5" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>127</v>
-      </c>
-      <c r="S5" t="s">
-        <v>129</v>
-      </c>
       <c r="T5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1718,67 +1721,67 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
         <v>136</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>137</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
         <v>139</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>140</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>141</v>
-      </c>
-      <c r="E3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
         <v>143</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>144</v>
-      </c>
-      <c r="D4" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1803,80 +1806,80 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="E1" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
         <v>146</v>
-      </c>
-      <c r="B2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
         <v>148</v>
-      </c>
-      <c r="B3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" t="s">
         <v>150</v>
-      </c>
-      <c r="B4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
         <v>152</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>153</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>154</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>155</v>
-      </c>
-      <c r="E5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
         <v>157</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>158</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>159</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>160</v>
-      </c>
-      <c r="E6" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1888,7 +1891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1907,213 +1910,213 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="Q1" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
         <v>163</v>
-      </c>
-      <c r="B2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" t="s">
-        <v>164</v>
       </c>
       <c r="F2"/>
       <c r="O2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" t="s">
         <v>169</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>167</v>
       </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" t="s">
         <v>171</v>
       </c>
-      <c r="E3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>174</v>
+      </c>
+      <c r="N3" t="s">
+        <v>173</v>
+      </c>
+      <c r="O3" t="s">
         <v>172</v>
-      </c>
-      <c r="J3" t="s">
-        <v>175</v>
-      </c>
-      <c r="N3" t="s">
-        <v>174</v>
-      </c>
-      <c r="O3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" t="s">
         <v>177</v>
       </c>
-      <c r="B4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" t="s">
         <v>178</v>
       </c>
-      <c r="F4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>179</v>
       </c>
-      <c r="I4" t="s">
+      <c r="N4" t="s">
+        <v>181</v>
+      </c>
+      <c r="O4" t="s">
         <v>180</v>
-      </c>
-      <c r="N4" t="s">
-        <v>182</v>
-      </c>
-      <c r="O4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
         <v>184</v>
       </c>
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H5" t="s">
         <v>185</v>
       </c>
-      <c r="F5" t="s">
-        <v>183</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" t="s">
+        <v>188</v>
+      </c>
+      <c r="O5" t="s">
         <v>187</v>
-      </c>
-      <c r="H5" t="s">
-        <v>186</v>
-      </c>
-      <c r="I5" t="s">
-        <v>100</v>
-      </c>
-      <c r="J5" t="s">
-        <v>190</v>
-      </c>
-      <c r="N5" t="s">
-        <v>189</v>
-      </c>
-      <c r="O5" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
         <v>192</v>
       </c>
-      <c r="B6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I6" t="s">
         <v>193</v>
       </c>
-      <c r="F6" t="s">
-        <v>168</v>
-      </c>
-      <c r="G6" t="s">
-        <v>168</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="N6" t="s">
         <v>194</v>
-      </c>
-      <c r="N6" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2138,16 +2141,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>13</v>
@@ -2155,145 +2158,145 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" t="s">
         <v>205</v>
-      </c>
-      <c r="C4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2319,19 +2322,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>69</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>13</v>
@@ -2339,87 +2342,87 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" t="s">
         <v>210</v>
       </c>
-      <c r="C2" t="s">
-        <v>211</v>
-      </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" t="s">
         <v>212</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>213</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>214</v>
-      </c>
-      <c r="E3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
         <v>216</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>217</v>
       </c>
-      <c r="D4" t="s">
-        <v>218</v>
-      </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" t="s">
         <v>219</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>220</v>
       </c>
-      <c r="D5" t="s">
-        <v>221</v>
-      </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" t="s">
         <v>222</v>
       </c>
-      <c r="C6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D6" t="s">
-        <v>223</v>
-      </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2443,69 +2446,69 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>76</v>
-      </c>
       <c r="J1" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
         <v>196</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
         <v>197</v>
       </c>
-      <c r="C2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>198</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>199</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H2" t="s">
         <v>200</v>
       </c>
-      <c r="G2" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" t="s">
         <v>201</v>
-      </c>
-      <c r="I2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J2" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2528,13 +2531,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
         <v>78</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolve compare issues (#70)
* Fix compare spreadsheet name normalization

Signed-off-by: Gary O'Neall <gary@sourceauditor.com>

* Additional checks for compares

- Check creator comment differences
- Check to make sure there are no duplicate document namespaces

Signed-off-by: Gary O'Neall <gary@sourceauditor.com>

* Remove temp file

Signed-off-by: Gary O'Neall <gary@sourceauditor.com>

* Update POM file with the latest library dependencies

Signed-off-by: Gary O'Neall <gary@sourceauditor.com>

* Use unique document URI's for all test files

Signed-off-by: Gary O'Neall <gary@sourceauditor.com>

Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/testResources/SPDXSpreadsheetExample-v2.3.xlsx
+++ b/testResources/SPDXSpreadsheetExample-v2.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary\git\tools-java\testResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3BF6B9-F289-4D2A-9372-956E20237E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54271B05-0BDD-4B4C-BDEE-CFA8EC64ED84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>2.3.0</t>
-  </si>
-  <si>
-    <t>http://spdx.org/spdxdocs/spdx-example-444504E0-4F89-41D3-9A0C-0305E82C3301</t>
   </si>
   <si>
     <t>Package Name</t>
@@ -806,6 +803,9 @@
   </si>
   <si>
     <t>Person: Package Commenter</t>
+  </si>
+  <si>
+    <t>http://spdx.org/spdxdocs/spdx-example-xlsx-2-3-444504E0-4F89-41D3-9A0C-0305E82C3301</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -973,6 +973,7 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,7 +1290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1357,53 +1360,53 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" t="s">
         <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" t="s">
-        <v>81</v>
       </c>
       <c r="L2" s="27">
         <v>40207.771087962959</v>
       </c>
       <c r="M2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="H3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="K4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1439,175 +1442,175 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" t="s">
-        <v>94</v>
       </c>
       <c r="D2"/>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
         <v>95</v>
-      </c>
-      <c r="I2" t="s">
-        <v>96</v>
       </c>
       <c r="J2"/>
       <c r="M2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>94</v>
+      </c>
+      <c r="T2" t="s">
         <v>95</v>
       </c>
-      <c r="N2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>95</v>
-      </c>
-      <c r="T2" t="s">
-        <v>96</v>
-      </c>
       <c r="U2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" t="s">
+        <v>101</v>
+      </c>
+      <c r="O3" t="s">
+        <v>107</v>
+      </c>
+      <c r="P3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q3" t="s">
         <v>99</v>
       </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="R3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" t="s">
         <v>116</v>
       </c>
-      <c r="H3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" t="s">
-        <v>104</v>
-      </c>
-      <c r="L3" t="s">
-        <v>111</v>
-      </c>
-      <c r="M3" t="s">
-        <v>101</v>
-      </c>
-      <c r="N3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P3" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>100</v>
-      </c>
-      <c r="R3" t="s">
-        <v>110</v>
-      </c>
-      <c r="S3" t="s">
-        <v>105</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>117</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>118</v>
-      </c>
-      <c r="W3" t="s">
-        <v>119</v>
       </c>
       <c r="X3" s="28">
         <v>40937.771087962959</v>
@@ -1621,80 +1624,80 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
         <v>120</v>
       </c>
-      <c r="B4" t="s">
-        <v>121</v>
-      </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4"/>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4"/>
       <c r="M4"/>
       <c r="N4"/>
       <c r="Q4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
         <v>125</v>
       </c>
-      <c r="B5" t="s">
-        <v>126</v>
-      </c>
       <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
         <v>134</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" t="s">
         <v>130</v>
-      </c>
-      <c r="G5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I5" t="s">
-        <v>131</v>
       </c>
       <c r="J5"/>
       <c r="M5" t="s">
+        <v>127</v>
+      </c>
+      <c r="N5" t="s">
+        <v>127</v>
+      </c>
+      <c r="P5" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>126</v>
+      </c>
+      <c r="S5" t="s">
         <v>128</v>
       </c>
-      <c r="N5" t="s">
-        <v>128</v>
-      </c>
-      <c r="P5" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>127</v>
-      </c>
-      <c r="S5" t="s">
-        <v>129</v>
-      </c>
       <c r="T5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1718,67 +1721,67 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
         <v>136</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>137</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
         <v>139</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>140</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>141</v>
-      </c>
-      <c r="E3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
         <v>143</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>144</v>
-      </c>
-      <c r="D4" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1803,80 +1806,80 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="E1" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
         <v>146</v>
-      </c>
-      <c r="B2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
         <v>148</v>
-      </c>
-      <c r="B3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" t="s">
         <v>150</v>
-      </c>
-      <c r="B4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
         <v>152</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>153</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>154</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>155</v>
-      </c>
-      <c r="E5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
         <v>157</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>158</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>159</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>160</v>
-      </c>
-      <c r="E6" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1888,7 +1891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1907,213 +1910,213 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="Q1" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
         <v>163</v>
-      </c>
-      <c r="B2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" t="s">
-        <v>164</v>
       </c>
       <c r="F2"/>
       <c r="O2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" t="s">
         <v>169</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>167</v>
       </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" t="s">
         <v>171</v>
       </c>
-      <c r="E3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>174</v>
+      </c>
+      <c r="N3" t="s">
+        <v>173</v>
+      </c>
+      <c r="O3" t="s">
         <v>172</v>
-      </c>
-      <c r="J3" t="s">
-        <v>175</v>
-      </c>
-      <c r="N3" t="s">
-        <v>174</v>
-      </c>
-      <c r="O3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" t="s">
         <v>177</v>
       </c>
-      <c r="B4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" t="s">
         <v>178</v>
       </c>
-      <c r="F4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>179</v>
       </c>
-      <c r="I4" t="s">
+      <c r="N4" t="s">
+        <v>181</v>
+      </c>
+      <c r="O4" t="s">
         <v>180</v>
-      </c>
-      <c r="N4" t="s">
-        <v>182</v>
-      </c>
-      <c r="O4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
         <v>184</v>
       </c>
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H5" t="s">
         <v>185</v>
       </c>
-      <c r="F5" t="s">
-        <v>183</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" t="s">
+        <v>188</v>
+      </c>
+      <c r="O5" t="s">
         <v>187</v>
-      </c>
-      <c r="H5" t="s">
-        <v>186</v>
-      </c>
-      <c r="I5" t="s">
-        <v>100</v>
-      </c>
-      <c r="J5" t="s">
-        <v>190</v>
-      </c>
-      <c r="N5" t="s">
-        <v>189</v>
-      </c>
-      <c r="O5" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
         <v>192</v>
       </c>
-      <c r="B6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I6" t="s">
         <v>193</v>
       </c>
-      <c r="F6" t="s">
-        <v>168</v>
-      </c>
-      <c r="G6" t="s">
-        <v>168</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="N6" t="s">
         <v>194</v>
-      </c>
-      <c r="N6" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2138,16 +2141,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>13</v>
@@ -2155,145 +2158,145 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" t="s">
         <v>205</v>
-      </c>
-      <c r="C4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2319,19 +2322,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>69</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>13</v>
@@ -2339,87 +2342,87 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" t="s">
         <v>210</v>
       </c>
-      <c r="C2" t="s">
-        <v>211</v>
-      </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" t="s">
         <v>212</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>213</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>214</v>
-      </c>
-      <c r="E3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
         <v>216</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>217</v>
       </c>
-      <c r="D4" t="s">
-        <v>218</v>
-      </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" t="s">
         <v>219</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>220</v>
       </c>
-      <c r="D5" t="s">
-        <v>221</v>
-      </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" t="s">
         <v>222</v>
       </c>
-      <c r="C6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D6" t="s">
-        <v>223</v>
-      </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2443,69 +2446,69 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>76</v>
-      </c>
       <c r="J1" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
         <v>196</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
         <v>197</v>
       </c>
-      <c r="C2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>198</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>199</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H2" t="s">
         <v>200</v>
       </c>
-      <c r="G2" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" t="s">
         <v>201</v>
-      </c>
-      <c r="I2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J2" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2528,13 +2531,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
         <v>78</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SPDX Java libraries to version 1.1.3
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/testResources/SPDXSpreadsheetExample-v2.3.xlsx
+++ b/testResources/SPDXSpreadsheetExample-v2.3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary\git\tools-java\testResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54271B05-0BDD-4B4C-BDEE-CFA8EC64ED84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DB1319-B511-4E20-B87D-90AB82ABA788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="228">
   <si>
     <t>Spreadsheet Version</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Primary Purpose</t>
+  </si>
+  <si>
+    <t>Release Date</t>
+  </si>
+  <si>
+    <t>Built Date</t>
+  </si>
+  <si>
+    <t>Valid Until Date</t>
   </si>
   <si>
     <t>User Defined Columns...</t>
@@ -356,7 +368,7 @@
 SHA256: 11b6d3ee554eedf79299905a98f9b9a04e498210b59f15094c916c91d150efcd</t>
   </si>
   <si>
-    <t>GPL-2.0-only,LicenseRef-2,LicenseRef-1</t>
+    <t>LicenseRef-2,GPL-2.0-only,LicenseRef-1</t>
   </si>
   <si>
     <t>The license for this project changed with the release of version x.y.  The version of the project included here post-dates the license change.</t>
@@ -452,7 +464,7 @@
     <t>OTHER</t>
   </si>
   <si>
-    <t>LocationRef-acmeforge</t>
+    <t>http://spdx.org/spdxdocs/spdx-example-444504E0-4F89-41D3-9A0C-0305E82C3301#LocationRef-acmeforge</t>
   </si>
   <si>
     <t>acmecorp/acmenator/4.1.3-alpha</t>
@@ -470,11 +482,11 @@
     <t>pkg:maven/org.apache.jena/apache-jena@3.12.0</t>
   </si>
   <si>
-    <t>LicenseRef-4</t>
+    <t>LicenseRef-1</t>
   </si>
   <si>
     <t>/*
- * (c) Copyright 2009 University of Bristol
+ * (c) Copyright 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009 Hewlett-Packard Development Company, LP
  * All rights reserved.
  *
  * Redistribution and use in source and binary forms, with or without
@@ -513,11 +525,11 @@
 THIS SOFTWARE IS PROVIDED BY THE AUTHOR ``AS IS'' AND ANY EXPRESS OR IMPLIED WARRANTIES, INCLUDING, BUT NOT LIMITED TO, THE IMPLIED WARRANTIES OF MERCHANTABILITY AND FITNESS FOR A PARTICULAR PURPOSE ARE DISCLAIMED. IN NO EVENT SHALL THE AUTHOR BE LIABLE FOR ANY DIRECT, INDIRECT, INCIDENTAL, SPECIAL, EXEMPLARY, OR CONSEQUENTIAL DAMAGES (INCLUDING, BUT NOT LIMITED TO, PROCUREMENT OF SUBSTITUTE GOODS OR SERVICES; LOSS OF USE, DATA, OR PROFITS; OR BUSINESS INTERRUPTION) HOWEVER CAUSED AND ON ANY THEORY OF LIABILITY, WHETHER IN CONTRACT, STRICT LIABILITY, OR TORT (INCLUDING NEGLIGENCE OR OTHERWISE) ARISING IN ANY WAY OUT OF THE USE OF THIS SOFTWARE, EVEN IF ADVISED OF THE POSSIBILITY OF SUCH DAMAGE.</t>
   </si>
   <si>
-    <t>LicenseRef-1</t>
+    <t>LicenseRef-4</t>
   </si>
   <si>
     <t>/*
- * (c) Copyright 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009 Hewlett-Packard Development Company, LP
+ * (c) Copyright 2009 University of Bristol
  * All rights reserved.
  *
  * Redistribution and use in source and binary forms, with or without
@@ -690,7 +702,7 @@
     <t>The concluded license was taken from the package level that the file was included in.</t>
   </si>
   <si>
-    <t>GPL-2.0-only, LicenseRef-2</t>
+    <t>LicenseRef-2, GPL-2.0-only</t>
   </si>
   <si>
     <t>The concluded license was taken from the package level that the file was included in.
@@ -805,14 +817,14 @@
     <t>Person: Package Commenter</t>
   </si>
   <si>
-    <t>http://spdx.org/spdxdocs/spdx-example-xlsx-2-3-444504E0-4F89-41D3-9A0C-0305E82C3301</t>
+    <t>http://spdx.org/spdxdocs/spdx-example-xlsx-2.3-444504E0-4F89-41D3-9A0C-0305E82C3301</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -865,6 +877,14 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -888,10 +908,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -905,77 +926,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1280,7 +1256,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1291,7 +1267,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1356,91 +1332,95 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>79</v>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="12">
+        <v>40207.771087962959</v>
+      </c>
+      <c r="M2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="H3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="K4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="H2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" t="s">
-        <v>85</v>
-      </c>
-      <c r="K2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L2" s="27">
-        <v>40207.771087962959</v>
-      </c>
-      <c r="M2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="K4" t="s">
-        <v>82</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{D1D5A5F6-EF9C-4C80-8372-015126BE0FE8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30" style="5" customWidth="1"/>
-    <col min="2" max="3" width="17" style="5" customWidth="1"/>
-    <col min="4" max="6" width="30" style="5" customWidth="1"/>
-    <col min="7" max="8" width="50" style="5" customWidth="1"/>
-    <col min="9" max="9" width="75" style="5" customWidth="1"/>
-    <col min="10" max="10" width="60" style="5" customWidth="1"/>
-    <col min="11" max="11" width="40" style="5" customWidth="1"/>
-    <col min="12" max="12" width="30" style="5" customWidth="1"/>
-    <col min="13" max="14" width="40" style="5" customWidth="1"/>
-    <col min="15" max="15" width="90" style="5" customWidth="1"/>
-    <col min="16" max="18" width="50" style="5" customWidth="1"/>
-    <col min="19" max="20" width="80" style="5" customWidth="1"/>
-    <col min="21" max="21" width="10" style="5" customWidth="1"/>
-    <col min="22" max="23" width="50" style="5" customWidth="1"/>
+    <col min="1" max="1" width="30" style="3" customWidth="1"/>
+    <col min="2" max="3" width="17" style="3" customWidth="1"/>
+    <col min="4" max="6" width="30" style="3" customWidth="1"/>
+    <col min="7" max="8" width="50" style="3" customWidth="1"/>
+    <col min="9" max="9" width="75" style="3" customWidth="1"/>
+    <col min="10" max="10" width="60" style="3" customWidth="1"/>
+    <col min="11" max="11" width="40" style="3" customWidth="1"/>
+    <col min="12" max="12" width="30" style="3" customWidth="1"/>
+    <col min="13" max="14" width="40" style="3" customWidth="1"/>
+    <col min="15" max="15" width="90" style="3" customWidth="1"/>
+    <col min="16" max="18" width="50" style="3" customWidth="1"/>
+    <col min="19" max="20" width="80" style="3" customWidth="1"/>
+    <col min="21" max="21" width="10" style="3" customWidth="1"/>
+    <col min="22" max="22" width="50" style="3" customWidth="1"/>
+    <col min="23" max="23" width="12" style="3" customWidth="1"/>
+    <col min="24" max="26" width="20" style="3" customWidth="1"/>
+    <col min="27" max="27" width="50" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -1510,194 +1490,209 @@
       <c r="W1" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2"/>
+      <c r="X1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="J2"/>
       <c r="M2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" t="s">
+        <v>99</v>
+      </c>
+      <c r="U2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="N2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>94</v>
-      </c>
-      <c r="T2" t="s">
-        <v>95</v>
-      </c>
-      <c r="U2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" t="s">
+        <v>114</v>
+      </c>
+      <c r="M3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" t="s">
         <v>112</v>
       </c>
-      <c r="D3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="Q3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" t="s">
         <v>113</v>
       </c>
-      <c r="G3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3" t="s">
-        <v>110</v>
-      </c>
-      <c r="M3" t="s">
-        <v>100</v>
-      </c>
-      <c r="N3" t="s">
-        <v>101</v>
-      </c>
-      <c r="O3" t="s">
-        <v>107</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>108</v>
       </c>
-      <c r="Q3" t="s">
-        <v>99</v>
-      </c>
-      <c r="R3" t="s">
-        <v>109</v>
-      </c>
-      <c r="S3" t="s">
-        <v>104</v>
-      </c>
       <c r="T3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="U3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="W3" t="s">
-        <v>118</v>
-      </c>
-      <c r="X3" s="28">
+        <v>122</v>
+      </c>
+      <c r="X3" s="12">
         <v>40937.771087962959</v>
       </c>
-      <c r="Y3" s="28">
+      <c r="Y3" s="12">
         <v>40572.771087962959</v>
       </c>
-      <c r="Z3" s="28">
+      <c r="Z3" s="12">
         <v>41668.771087962959</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
+    <row r="4" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="D4"/>
       <c r="G4" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="J4"/>
-      <c r="M4"/>
-      <c r="N4"/>
+      <c r="M4" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" t="s">
+        <v>98</v>
+      </c>
       <c r="Q4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="T4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="U4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" t="s">
         <v>133</v>
       </c>
-      <c r="D5" t="s">
-        <v>129</v>
-      </c>
       <c r="G5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" t="s">
         <v>134</v>
-      </c>
-      <c r="H5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" t="s">
-        <v>130</v>
       </c>
       <c r="J5"/>
       <c r="M5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="N5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="P5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="Q5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="S5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="T5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="U5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1713,75 +1708,75 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="25" style="7" customWidth="1"/>
-    <col min="3" max="3" width="40" style="8" customWidth="1"/>
-    <col min="4" max="4" width="60" style="8" customWidth="1"/>
-    <col min="5" max="6" width="40" style="8" customWidth="1"/>
+    <col min="1" max="2" width="25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40" style="3" customWidth="1"/>
+    <col min="4" max="4" width="60" style="3" customWidth="1"/>
+    <col min="5" max="6" width="40" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C2" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D2" s="3" t="s">
         <v>141</v>
       </c>
     </row>
+    <row r="3" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" t="s">
-        <v>144</v>
+      <c r="A4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1797,89 +1792,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15" style="10" customWidth="1"/>
+    <col min="1" max="1" width="15" style="2" customWidth="1"/>
     <col min="2" max="2" width="120" customWidth="1"/>
-    <col min="3" max="3" width="50" style="10" customWidth="1"/>
-    <col min="4" max="5" width="80" style="11" customWidth="1"/>
-    <col min="6" max="6" width="50" style="11" customWidth="1"/>
+    <col min="3" max="3" width="50" style="2" customWidth="1"/>
+    <col min="4" max="5" width="80" style="3" customWidth="1"/>
+    <col min="6" max="6" width="50" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>36</v>
+      <c r="F1" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>145</v>
+      <c r="A2" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>147</v>
+      <c r="A3" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>149</v>
+      <c r="A4" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>151</v>
+      <c r="A5" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>156</v>
+      <c r="A6" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E6" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1891,150 +1886,150 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="60" style="14" customWidth="1"/>
-    <col min="2" max="3" width="25" style="13" customWidth="1"/>
-    <col min="4" max="4" width="30" style="14" customWidth="1"/>
-    <col min="5" max="5" width="85" style="14" customWidth="1"/>
-    <col min="6" max="7" width="50" style="14" customWidth="1"/>
-    <col min="8" max="8" width="60" style="14" customWidth="1"/>
-    <col min="9" max="10" width="70" style="14" customWidth="1"/>
-    <col min="11" max="11" width="35" style="14" customWidth="1"/>
-    <col min="12" max="18" width="60" style="14" customWidth="1"/>
+    <col min="1" max="1" width="60" style="3" customWidth="1"/>
+    <col min="2" max="3" width="25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30" style="3" customWidth="1"/>
+    <col min="5" max="5" width="85" style="3" customWidth="1"/>
+    <col min="6" max="7" width="50" style="3" customWidth="1"/>
+    <col min="8" max="8" width="60" style="3" customWidth="1"/>
+    <col min="9" max="10" width="70" style="3" customWidth="1"/>
+    <col min="11" max="11" width="35" style="3" customWidth="1"/>
+    <col min="12" max="18" width="60" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="I1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="J1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="K1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="L1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="M1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="12" t="s">
-        <v>36</v>
+      <c r="R1" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>162</v>
+      <c r="A2" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2"/>
+        <v>167</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
       <c r="O2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="J3" t="s">
+        <v>178</v>
+      </c>
+      <c r="N3" t="s">
+        <v>177</v>
+      </c>
+      <c r="O3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
         <v>174</v>
       </c>
-      <c r="N3" t="s">
-        <v>173</v>
-      </c>
-      <c r="O3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" t="s">
-        <v>170</v>
-      </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F4" t="s">
         <v>149</v>
@@ -2043,80 +2038,80 @@
         <v>149</v>
       </c>
       <c r="H4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="I4" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="N4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="O4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>183</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="150" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G5" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H5" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="J5" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="N5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="O5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
         <v>191</v>
       </c>
+    </row>
+    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F6" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G6" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="N6" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2132,171 +2127,171 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20" style="16" customWidth="1"/>
-    <col min="2" max="2" width="25" style="16" customWidth="1"/>
-    <col min="3" max="3" width="20" style="16" customWidth="1"/>
-    <col min="4" max="4" width="70" style="17" customWidth="1"/>
-    <col min="5" max="5" width="50" style="17" customWidth="1"/>
+    <col min="1" max="1" width="20" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20" style="2" customWidth="1"/>
+    <col min="4" max="4" width="70" style="3" customWidth="1"/>
+    <col min="5" max="5" width="50" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="A1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" t="s">
-        <v>90</v>
-      </c>
-    </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C4" t="s">
-        <v>205</v>
+      <c r="A4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C7" t="s">
-        <v>120</v>
+      <c r="C7" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" t="s">
-        <v>203</v>
-      </c>
-      <c r="C8" t="s">
-        <v>90</v>
+      <c r="A8" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" t="s">
-        <v>203</v>
-      </c>
-      <c r="C9" t="s">
-        <v>166</v>
+      <c r="A9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C10" t="s">
-        <v>190</v>
+      <c r="A10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" t="s">
-        <v>203</v>
-      </c>
-      <c r="C11" t="s">
-        <v>175</v>
+      <c r="A11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C12" t="s">
-        <v>161</v>
+      <c r="A12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" t="s">
-        <v>207</v>
-      </c>
-      <c r="C13" t="s">
-        <v>125</v>
+      <c r="A13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C14" t="s">
-        <v>120</v>
+      <c r="A14" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2312,117 +2307,117 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25" style="19" customWidth="1"/>
-    <col min="2" max="2" width="70" style="20" customWidth="1"/>
-    <col min="3" max="3" width="25" style="19" customWidth="1"/>
-    <col min="4" max="4" width="60" style="20" customWidth="1"/>
-    <col min="5" max="5" width="20" style="19" customWidth="1"/>
-    <col min="6" max="6" width="50" style="20" customWidth="1"/>
+    <col min="1" max="1" width="25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="70" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="60" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20" style="2" customWidth="1"/>
+    <col min="6" max="6" width="50" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="A1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="B1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C2" s="2" t="s">
         <v>214</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C4" t="s">
-        <v>216</v>
-      </c>
-      <c r="D4" t="s">
-        <v>217</v>
-      </c>
-      <c r="E4" t="s">
-        <v>214</v>
+      <c r="A4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C5" t="s">
-        <v>219</v>
-      </c>
-      <c r="D5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E5" t="s">
-        <v>138</v>
+      <c r="A5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D6" t="s">
-        <v>222</v>
-      </c>
-      <c r="E6" t="s">
-        <v>138</v>
+      <c r="A6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2438,77 +2433,77 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="25" style="22" customWidth="1"/>
-    <col min="4" max="5" width="40" style="22" customWidth="1"/>
-    <col min="6" max="10" width="60" style="23" customWidth="1"/>
-    <col min="11" max="11" width="40" style="23" customWidth="1"/>
+    <col min="1" max="3" width="25" style="2" customWidth="1"/>
+    <col min="4" max="5" width="40" style="2" customWidth="1"/>
+    <col min="6" max="10" width="60" style="3" customWidth="1"/>
+    <col min="11" max="11" width="40" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="B1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="B2" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="I2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>201</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2524,20 +2519,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="60" style="26" customWidth="1"/>
-    <col min="2" max="2" width="20" style="25" customWidth="1"/>
-    <col min="3" max="3" width="120" style="26" customWidth="1"/>
+    <col min="1" max="1" width="60" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20" style="2" customWidth="1"/>
+    <col min="3" max="3" width="120" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>78</v>
+      <c r="A1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>